<commit_message>
Updated excel file for 10x_xenium_mouse_pup_preview dataset
</commit_message>
<xml_diff>
--- a/datasets/10x_xenium_mouse_pup_preview.xlsx
+++ b/datasets/10x_xenium_mouse_pup_preview.xlsx
@@ -61,13 +61,13 @@
     <t xml:space="preserve">RNA,ControlCodeword,ControlProbe,BlankCodeword</t>
   </si>
   <si>
-    <t xml:space="preserve">datasets/10x_xenium_mouse_pup_preview/filtered_feature_bc_matrix.h5</t>
+    <t xml:space="preserve">datasets/10x_xenium_mouse_pup_preview/cell_feature_matrix.h5</t>
   </si>
   <si>
     <t xml:space="preserve">datasets/10x_xenium_mouse_pup_preview/metrics_summary.csv</t>
   </si>
   <si>
-    <t xml:space="preserve">datasets/10x_xenium_mouse_pup_preview/analysis/kmeans/10_clusters/clusters.csv</t>
+    <t xml:space="preserve">datasets/10x_xenium_mouse_pup_preview/analysis/clustering/gene_expression_kmeans_10_clusters/clusters.csv</t>
   </si>
   <si>
     <t xml:space="preserve">ENSEMBL,NO,NO,NO</t>
@@ -173,10 +173,10 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.56"/>
   </cols>

</xml_diff>